<commit_message>
Titles for files added
</commit_message>
<xml_diff>
--- a/govHackKeywords.xlsx
+++ b/govHackKeywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37051ee2c1ee6dec/Documents/GitHub/GovHack 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanushp/Documents/GitHub/InfluenzAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{777E48F7-06B0-4A23-9F36-B2BA8E1EBB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{042485D5-ED54-478F-86DA-6AA43EE09705}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93868E81-0C13-2E42-B9B7-8F58E6F8166D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="4392" windowWidth="20808" windowHeight="9960" xr2:uid="{7127F0B4-DC6C-4E99-B4C0-5D92909B69EF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7127F0B4-DC6C-4E99-B4C0-5D92909B69EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Document</t>
   </si>
@@ -211,13 +211,91 @@
   </si>
   <si>
     <t>https://www.aihw.gov.au/getmedia/f451fcb7-be85-401c-8e3d-efd815be84e6/aihw-aus-240_Chapter_3.pdf.aspx</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Acute rheumatic conditions</t>
+  </si>
+  <si>
+    <t>Communicable diseases intelligence</t>
+  </si>
+  <si>
+    <t>Clinical and translational Immunology</t>
+  </si>
+  <si>
+    <t>Covid 19: second report</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 9</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 8</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 7</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 6</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 5</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 4</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 3</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 2</t>
+  </si>
+  <si>
+    <t>Influenza surveillance report 1</t>
+  </si>
+  <si>
+    <t>Pneumonia using Bayesian network</t>
+  </si>
+  <si>
+    <t>Communicable diseases intelligence 2011-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasonal Influenza Infection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respiratory Infection in Residential Care </t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates Aug</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates Jul 1</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates Jul 2</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates Jun 2</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates Jun 1</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates May 2</t>
+  </si>
+  <si>
+    <t>Covid 19 Vaccine Rates May 1</t>
+  </si>
+  <si>
+    <t>Survey for influenza vaccination in young adults</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +307,24 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,12 +351,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -576,455 +674,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0C90F4-C831-4DE3-BF01-D5C9DD5107A2}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="219" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="109.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="109.5" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
       <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
       <c r="D12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
       <c r="D13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
       <c r="D14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
       <c r="D18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
       <c r="D21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
       <c r="D23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
       <c r="D24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>44</v>
       </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
       <c r="D25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>53</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>54</v>
       </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>54</v>
       </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>20</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>54</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{3F5105E4-21AD-49F9-AB37-09D804E8564F}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{BCAC58CA-6457-410E-BECE-7E81B6D68B65}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{3F5105E4-21AD-49F9-AB37-09D804E8564F}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{BCAC58CA-6457-410E-BECE-7E81B6D68B65}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{AE212279-180D-304C-B6C8-07294594EA97}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{3D1B9E80-24A8-9942-B63B-68590DA09D9F}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{DD531C19-8458-144C-98C6-6B7F83E5F2C2}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{5723324A-7189-E34F-9764-CDC707064E33}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{EEC1D3F9-5C77-E84A-B7B1-89C3BF1DB5FD}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{D8E58ECA-8C4D-734A-8A2E-3244BE79DD0A}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{A7091CA9-67D0-D949-9394-BA118A89A252}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{164A041C-44D4-A949-ADB2-C9B09BA24D94}"/>
+    <hyperlink ref="B19" r:id="rId11" xr:uid="{D6893E74-6150-794F-B5D9-63878D0F3516}"/>
+    <hyperlink ref="B26" r:id="rId12" xr:uid="{F7A7F573-F2C0-E14F-B3DE-82CE1B2765A4}"/>
+    <hyperlink ref="B27" r:id="rId13" xr:uid="{2CB7212B-E99E-034F-AA1F-21EC335E4F09}"/>
+    <hyperlink ref="B28" r:id="rId14" xr:uid="{ACF61E56-D782-5647-898D-C31C28D59B20}"/>
+    <hyperlink ref="B29" r:id="rId15" xr:uid="{193FAA7D-6E4B-9145-B409-89D463B1B531}"/>
+    <hyperlink ref="B30" r:id="rId16" xr:uid="{6A8F98D0-960B-8145-B409-FFB591620A20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>